<commit_message>
add table design and process
</commit_message>
<xml_diff>
--- a/public/需求总览.xlsx
+++ b/public/需求总览.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\learn\public\upload\requireFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\learn\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49F8C88-EA56-4469-B4F1-DAB2263B5EA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00F5B30-03E8-4754-9144-9960A3C8B339}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="大鹏需求总览" sheetId="1" r:id="rId1"/>
     <sheet name="管理需求" sheetId="2" r:id="rId2"/>
+    <sheet name="管理课程作品作业动态" sheetId="3" r:id="rId3"/>
+    <sheet name="后台数据表详情" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>大分类</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -277,6 +280,18 @@
   </si>
   <si>
     <t>二级</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>课程管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理课程/作品/作业/动态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后台数据存储设计</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -284,7 +299,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,15 +315,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="10"/>
       <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -344,10 +375,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -355,28 +387,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -389,6 +430,122 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>39461</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4649AB7D-59EA-4F51-8A22-F1CEA0A795EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685799" y="114301"/>
+          <a:ext cx="8105775" cy="10421710"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7B54AB6-E812-4218-B7E3-E3348162EB57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="923925" y="104775"/>
+          <a:ext cx="6238875" cy="9344025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -654,15 +811,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.25" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
     <col min="3" max="3" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -675,135 +832,135 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5" t="str">
+      <c r="A17" s="11"/>
+      <c r="B17" s="6" t="str">
         <f>"走进"&amp;A1</f>
         <v>走进大鹏</v>
       </c>
@@ -811,171 +968,171 @@
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="11"/>
+      <c r="B23" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="5" t="s">
+      <c r="A24" s="11"/>
+      <c r="B24" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="5" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="11"/>
+      <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="11"/>
+      <c r="B30" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="11"/>
+      <c r="B31" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="11"/>
+      <c r="B32" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="11"/>
+      <c r="B33" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="11"/>
+      <c r="B34" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="11"/>
+      <c r="B36" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="6" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -983,32 +1140,32 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="3"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="3"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="3"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="11"/>
+      <c r="B41" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -1016,28 +1173,28 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="6"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="6"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="6"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -1045,49 +1202,49 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
+      <c r="A46" s="11"/>
       <c r="B46" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
+      <c r="A47" s="11"/>
       <c r="B47" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
+      <c r="A48" s="11"/>
       <c r="B48" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
+      <c r="A49" s="11"/>
       <c r="B49" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B53" s="7" t="s">
@@ -1095,30 +1252,45 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
+      <c r="A55" s="11"/>
       <c r="B55" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="A56" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="A57" s="10" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A45:A52"/>
     <mergeCell ref="A53:A55"/>
     <mergeCell ref="A3:A21"/>
     <mergeCell ref="A22:A25"/>
@@ -1127,8 +1299,13 @@
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="B41:B44"/>
     <mergeCell ref="A35:A44"/>
+    <mergeCell ref="A45:A52"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B58" location="管理课程作品作业动态!A1" display="管理课程/作品/作业/动态" xr:uid="{60618750-3F22-4447-82A0-8551D59F7BD0}"/>
+    <hyperlink ref="B59" location="后台数据表详情!A1" display="后台数据存储设计" xr:uid="{4322BA8F-4B6C-479C-9D48-6D28BC8A78F2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1138,7 +1315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793E50C3-656F-4911-A3F1-451866435E5B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -1147,4 +1324,1865 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB216836-B1F3-489D-8ED9-D422FF4F3C18}">
+  <dimension ref="A1:O60"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5494EB0B-EDC8-47A4-831C-C03A1D975028}">
+  <dimension ref="A1:M53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCED2D15-4BE7-4BEB-A594-ECB8C976C978}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>